<commit_message>
Append w/ format test
</commit_message>
<xml_diff>
--- a/sch.xlsx
+++ b/sch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohamedselim\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\Python\Projects\sch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702D107E-FCA9-44DF-A34E-B621EE7DD9B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD822C9E-C435-4FE1-AF24-72E4566B128B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BECA3ED2-DCF8-4224-8D9F-5B5D9782EAE2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{BECA3ED2-DCF8-4224-8D9F-5B5D9782EAE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>From</t>
   </si>
@@ -54,15 +54,28 @@
     <t>Target hrs/day, week, month</t>
   </si>
   <si>
-    <t>0/1/1900  1:00:00 AM</t>
+    <t>6/13/22  8:00 AM</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="170" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -111,11 +124,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
-    <xf numFmtId="168" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -431,17 +458,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A611A7-1354-4CC5-B404-EFA3A30F9B70}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -454,7 +480,7 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -465,14 +491,56 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C2" s="3">
+        <f ca="1">NOW()</f>
+        <v>44725.883369328702</v>
+      </c>
+      <c r="D2" s="5">
+        <f ca="1">C2-B2</f>
+        <v>44725.550035995366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="3">
+        <f>TIME( 1, 2, 3)</f>
+        <v>4.3090277777777776E-2</v>
+      </c>
       <c r="I4" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="3">
+        <v>36892.041666666664</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="5"/>
+      <c r="I11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>